<commit_message>
Added docs and slides.
</commit_message>
<xml_diff>
--- a/docs/stm-heap-perf.xlsx
+++ b/docs/stm-heap-perf.xlsx
@@ -261,11 +261,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1287969774"/>
-        <c:axId val="1359299837"/>
+        <c:axId val="1022534844"/>
+        <c:axId val="611170046"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1287969774"/>
+        <c:axId val="1022534844"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -297,10 +297,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1359299837"/>
+        <c:crossAx val="611170046"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1359299837"/>
+        <c:axId val="611170046"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -349,7 +349,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1287969774"/>
+        <c:crossAx val="1022534844"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -516,11 +516,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="909867232"/>
-        <c:axId val="254663032"/>
+        <c:axId val="1558176819"/>
+        <c:axId val="1339704777"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="909867232"/>
+        <c:axId val="1558176819"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -552,10 +552,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="254663032"/>
+        <c:crossAx val="1339704777"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="254663032"/>
+        <c:axId val="1339704777"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -604,7 +604,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="909867232"/>
+        <c:crossAx val="1558176819"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -668,11 +668,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1794953290"/>
-        <c:axId val="442850392"/>
+        <c:axId val="2138333606"/>
+        <c:axId val="1172100704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1794953290"/>
+        <c:axId val="2138333606"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -704,10 +704,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="442850392"/>
+        <c:crossAx val="1172100704"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442850392"/>
+        <c:axId val="1172100704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -756,7 +756,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1794953290"/>
+        <c:crossAx val="2138333606"/>
       </c:valAx>
     </c:plotArea>
   </c:chart>

</xml_diff>